<commit_message>
updated the activity status
</commit_message>
<xml_diff>
--- a/Planing/PyramidRecruiterDashboard.xlsx
+++ b/Planing/PyramidRecruiterDashboard.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="105">
   <si>
     <t>Activity</t>
   </si>
@@ -355,6 +355,12 @@
   </si>
   <si>
     <t>Password: adminadmin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Done </t>
+  </si>
+  <si>
+    <t>Partialy Done</t>
   </si>
 </sst>
 </file>
@@ -755,7 +761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -811,7 +817,9 @@
         <v>44</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H2" s="5" t="s">
         <v>69</v>
       </c>
@@ -827,7 +835,9 @@
         <v>45</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -841,7 +851,9 @@
         <v>45</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -856,10 +868,12 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H5" s="5" t="s">
         <v>70</v>
       </c>
@@ -877,7 +891,9 @@
       <c r="F6" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -893,7 +909,9 @@
         <v>44</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -907,7 +925,9 @@
         <v>44</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -920,10 +940,12 @@
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -934,10 +956,12 @@
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -948,12 +972,14 @@
         <v>20</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -964,10 +990,12 @@
         <v>21</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -983,7 +1011,9 @@
         <v>45</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -996,10 +1026,12 @@
         <v>23</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1017,7 +1049,9 @@
         <v>46</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="H15" s="5" t="s">
         <v>71</v>
       </c>
@@ -1035,7 +1069,9 @@
       <c r="F16" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1051,7 +1087,9 @@
         <v>45</v>
       </c>
       <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1065,7 +1103,9 @@
         <v>45</v>
       </c>
       <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1081,7 +1121,9 @@
         <v>47</v>
       </c>
       <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1095,7 +1137,9 @@
         <v>47</v>
       </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H20" s="6"/>
     </row>
     <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1111,7 +1155,9 @@
       <c r="F21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1125,7 +1171,9 @@
         <v>47</v>
       </c>
       <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1333,7 +1381,9 @@
         <v>54</v>
       </c>
       <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+      <c r="G35" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1347,7 +1397,9 @@
         <v>54</v>
       </c>
       <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1365,7 +1417,9 @@
         <v>73</v>
       </c>
       <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
+      <c r="G37" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1379,7 +1433,9 @@
         <v>73</v>
       </c>
       <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="G38" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1395,7 +1451,9 @@
       <c r="F39" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G39" s="2"/>
+      <c r="G39" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1446,7 +1504,7 @@
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H42" s="2"/>
     </row>
@@ -1505,7 +1563,9 @@
         <v>63</v>
       </c>
       <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
+      <c r="G46" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1549,7 +1609,9 @@
       <c r="F49" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G49" s="2"/>
+      <c r="G49" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="H49" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added few more QA tasks
</commit_message>
<xml_diff>
--- a/Planing/PyramidRecruiterDashboard.xlsx
+++ b/Planing/PyramidRecruiterDashboard.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="108">
   <si>
     <t>Activity</t>
   </si>
@@ -361,6 +361,15 @@
   </si>
   <si>
     <t>Partialy Done</t>
+  </si>
+  <si>
+    <t>Bussiness Requirement Creation</t>
+  </si>
+  <si>
+    <t>Test Plan</t>
+  </si>
+  <si>
+    <t>Automation Framework set-up</t>
   </si>
 </sst>
 </file>
@@ -759,9 +768,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1438,37 +1449,31 @@
       </c>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>75</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="F39" s="2"/>
       <c r="G39" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
-        <v>8</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2" t="s">
@@ -1480,11 +1485,11 @@
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2" t="s">
@@ -1492,63 +1497,73 @@
       </c>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F42" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="G42" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
+      <c r="A43" s="2">
+        <v>8</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="C43" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
+      <c r="G43" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
+      <c r="G44" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H45" s="2"/>
     </row>
@@ -1556,63 +1571,107 @@
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F46" s="2"/>
-      <c r="G46" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
+      <c r="G48" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F52" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="G52" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="H49" s="2"/>
+      <c r="H52" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>